<commit_message>
Changement des noms des graphique.
</commit_message>
<xml_diff>
--- a/Documents/DocumentationGenerale/PID_Comportement.xlsx
+++ b/Documents/DocumentationGenerale/PID_Comportement.xlsx
@@ -450,6 +450,10 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -459,6 +463,9 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>I</c:v>
+          </c:tx>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
@@ -773,7 +780,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Derivation</c:v>
+            <c:v>D</c:v>
           </c:tx>
           <c:marker>
             <c:symbol val="none"/>
@@ -1391,6 +1398,10 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout>
@@ -1410,6 +1421,9 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>PID</c:v>
+          </c:tx>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
@@ -2175,8 +2189,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>